<commit_message>
Project Goal Analysis Report
</commit_message>
<xml_diff>
--- a/ProjectGoalAnalysis.xlsx
+++ b/ProjectGoalAnalysis.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shahp\Documents\GitHub\PacWoman\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9210848A-92B9-474F-8DB3-C7B723563DAA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A9EBF11-AAA6-4700-A281-A7D0DCD534F2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E67C6D3D-A769-4404-BC41-B3C51D88A6CC}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{E67C6D3D-A769-4404-BC41-B3C51D88A6CC}"/>
   </bookViews>
   <sheets>
     <sheet name="ProjectStatusReport" sheetId="1" r:id="rId1"/>
+    <sheet name="BackerStatusReport" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -1904,8 +1905,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77813A8B-F3A5-4122-8133-C7B6B8D3BDAB}">
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2311,4 +2312,16 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{592CCCE7-2EAD-424A-A788-FF446134280F}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>